<commit_message>
project results and repo cleanup
</commit_message>
<xml_diff>
--- a/ai-nano/projects/3-planning/results/data-table.xlsx
+++ b/ai-nano/projects/3-planning/results/data-table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
   <si>
     <t>Problem 1</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Problem 3</t>
+  </si>
+  <si>
+    <t>timeout</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +121,20 @@
       <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -284,6 +301,15 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,7 +591,7 @@
   <dimension ref="B1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,135 +891,235 @@
       <c r="C16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="11"/>
+      <c r="D16" s="6">
+        <v>205</v>
+      </c>
+      <c r="E16" s="6">
+        <v>337</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1317</v>
+      </c>
+      <c r="G16" s="6">
+        <v>6</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0.545943581004394</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="15"/>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="11"/>
+      <c r="D17" s="6">
+        <v>19747</v>
+      </c>
+      <c r="E17" s="6">
+        <v>19748</v>
+      </c>
+      <c r="F17" s="6">
+        <v>108950</v>
+      </c>
+      <c r="G17" s="6">
+        <v>6</v>
+      </c>
+      <c r="H17" s="11">
+        <v>41.108592712000203</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="11"/>
+      <c r="D18" s="6">
+        <v>14</v>
+      </c>
+      <c r="E18" s="6">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6">
+        <v>41</v>
+      </c>
+      <c r="G18" s="6">
+        <v>9</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1.6682864006725098E-2</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="11"/>
+      <c r="D19" s="6">
+        <v>1392</v>
+      </c>
+      <c r="E19" s="6">
+        <v>8572</v>
+      </c>
+      <c r="F19" s="6">
+        <v>8959</v>
+      </c>
+      <c r="G19" s="6">
+        <v>50</v>
+      </c>
+      <c r="H19" s="11">
+        <v>4.8224815459980102</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="11"/>
+      <c r="D20" s="6">
+        <v>387</v>
+      </c>
+      <c r="E20" s="6">
+        <v>389</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2351</v>
+      </c>
+      <c r="G20" s="6">
+        <v>6</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0.87828166900726501</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="11"/>
+      <c r="D21" s="6">
+        <v>84055</v>
+      </c>
+      <c r="E21" s="6">
+        <v>84056</v>
+      </c>
+      <c r="F21" s="6">
+        <v>445019</v>
+      </c>
+      <c r="G21" s="6">
+        <v>6</v>
+      </c>
+      <c r="H21" s="11">
+        <v>168.35773514299899</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
       <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="11"/>
+      <c r="D22" s="6">
+        <v>193</v>
+      </c>
+      <c r="E22" s="6">
+        <v>195</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1026</v>
+      </c>
+      <c r="G22" s="6">
+        <v>10</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0.39227325099636801</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="11"/>
+      <c r="D23" s="6">
+        <v>387</v>
+      </c>
+      <c r="E23" s="6">
+        <v>389</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2351</v>
+      </c>
+      <c r="G23" s="6">
+        <v>6</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0.86623552899982303</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
       <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="11"/>
+      <c r="D24" s="6">
+        <v>108</v>
+      </c>
+      <c r="E24" s="6">
+        <v>110</v>
+      </c>
+      <c r="F24" s="6">
+        <v>761</v>
+      </c>
+      <c r="G24" s="6">
+        <v>6</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0.28954632999375401</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
       <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="11"/>
+      <c r="D25" s="6">
+        <v>35</v>
+      </c>
+      <c r="E25" s="6">
+        <v>37</v>
+      </c>
+      <c r="F25" s="6">
+        <v>192</v>
+      </c>
+      <c r="G25" s="6">
+        <v>6</v>
+      </c>
+      <c r="H25" s="11">
+        <v>33.2912620179995</v>
+      </c>
     </row>
     <row r="26" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="9" t="e">
+      <c r="D26" s="9">
         <f>AVERAGE(D16:D25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="9" t="e">
+        <v>10652.3</v>
+      </c>
+      <c r="E26" s="9">
         <f t="shared" ref="E26" si="1">AVERAGE(E16:E25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="17" t="e">
+        <v>11384.8</v>
+      </c>
+      <c r="F26" s="17">
         <f t="shared" ref="F26" si="2">AVERAGE(F16:F25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="17" t="e">
+        <v>57096.7</v>
+      </c>
+      <c r="G26" s="17">
         <f t="shared" ref="G26" si="3">AVERAGE(G16:G25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="10" t="e">
+        <v>11.1</v>
+      </c>
+      <c r="H26" s="10">
         <f t="shared" ref="H26" si="4">AVERAGE(H16:H25)</f>
-        <v>#DIV/0!</v>
+        <v>25.0569034643005</v>
       </c>
     </row>
     <row r="28" spans="2:8" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1024,40 +1150,64 @@
       <c r="C29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="11"/>
+      <c r="D29" s="6">
+        <v>14491</v>
+      </c>
+      <c r="E29" s="6">
+        <v>17947</v>
+      </c>
+      <c r="F29" s="6">
+        <v>128184</v>
+      </c>
+      <c r="G29" s="6">
+        <v>12</v>
+      </c>
+      <c r="H29" s="11">
+        <v>131.446662653994</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
       <c r="C30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="11"/>
+      <c r="D30" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
       <c r="C31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="11"/>
+      <c r="D31" s="6">
+        <v>1948</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1949</v>
+      </c>
+      <c r="F31" s="6">
+        <v>16253</v>
+      </c>
+      <c r="G31" s="6">
+        <v>1878</v>
+      </c>
+      <c r="H31" s="11">
+        <v>26.679062017996301</v>
+      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
       <c r="C32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -1068,18 +1218,30 @@
       <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="11"/>
+      <c r="D33" s="6">
+        <v>17783</v>
+      </c>
+      <c r="E33" s="6">
+        <v>17785</v>
+      </c>
+      <c r="F33" s="6">
+        <v>155920</v>
+      </c>
+      <c r="G33" s="6">
+        <v>12</v>
+      </c>
+      <c r="H33" s="11">
+        <v>64.015925721003399</v>
+      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
       <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -1090,40 +1252,72 @@
       <c r="C35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="11"/>
+      <c r="D35" s="6">
+        <v>4031</v>
+      </c>
+      <c r="E35" s="6">
+        <v>4033</v>
+      </c>
+      <c r="F35" s="6">
+        <v>35794</v>
+      </c>
+      <c r="G35" s="6">
+        <v>22</v>
+      </c>
+      <c r="H35" s="11">
+        <v>15.8658084640046</v>
+      </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
       <c r="C36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="11"/>
+      <c r="D36" s="6">
+        <v>17783</v>
+      </c>
+      <c r="E36" s="6">
+        <v>17785</v>
+      </c>
+      <c r="F36" s="6">
+        <v>155920</v>
+      </c>
+      <c r="G36" s="6">
+        <v>12</v>
+      </c>
+      <c r="H36" s="11">
+        <v>62.893093974998898</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
       <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="11"/>
+      <c r="D37" s="6">
+        <v>5003</v>
+      </c>
+      <c r="E37" s="6">
+        <v>5005</v>
+      </c>
+      <c r="F37" s="6">
+        <v>44586</v>
+      </c>
+      <c r="G37" s="6">
+        <v>12</v>
+      </c>
+      <c r="H37" s="11">
+        <v>19.118624861992402</v>
+      </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="15"/>
       <c r="C38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="6"/>
+      <c r="D38" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -1134,25 +1328,25 @@
       <c r="C39" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="9" t="e">
+      <c r="D39" s="9">
         <f>AVERAGE(D29:D38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E39" s="9" t="e">
+        <v>10173.166666666666</v>
+      </c>
+      <c r="E39" s="9">
         <f t="shared" ref="E39" si="5">AVERAGE(E29:E38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F39" s="17" t="e">
+        <v>10750.666666666666</v>
+      </c>
+      <c r="F39" s="17">
         <f t="shared" ref="F39" si="6">AVERAGE(F29:F38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G39" s="17" t="e">
+        <v>89442.833333333328</v>
+      </c>
+      <c r="G39" s="17">
         <f t="shared" ref="G39" si="7">AVERAGE(G29:G38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H39" s="10" t="e">
+        <v>324.66666666666669</v>
+      </c>
+      <c r="H39" s="10">
         <f t="shared" ref="H39" si="8">AVERAGE(H29:H38)</f>
-        <v>#DIV/0!</v>
+        <v>53.336529615664936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated results data tables
</commit_message>
<xml_diff>
--- a/ai-nano/projects/3-planning/results/data-table.xlsx
+++ b/ai-nano/projects/3-planning/results/data-table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16120" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18500" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>Problem 1</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>timeout</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -97,9 +106,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +146,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -253,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -275,15 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -305,11 +312,32 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,753 +627,841 @@
     <col min="1" max="1" width="4.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" style="2" customWidth="1"/>
-    <col min="4" max="8" width="14.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="9" width="13.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6">
         <v>43</v>
       </c>
-      <c r="E3" s="6">
+      <c r="G3" s="6">
         <v>56</v>
       </c>
-      <c r="F3" s="6">
+      <c r="H3" s="6">
         <v>180</v>
       </c>
-      <c r="G3" s="6">
-        <v>6</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="I3" s="18">
         <v>4.0883048997784499E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="15"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="12"/>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6">
         <v>1458</v>
       </c>
-      <c r="E4" s="6">
+      <c r="G4" s="6">
         <v>1459</v>
       </c>
-      <c r="F4" s="6">
+      <c r="H4" s="6">
         <v>5960</v>
       </c>
-      <c r="G4" s="6">
-        <v>6</v>
-      </c>
-      <c r="H4" s="11">
+      <c r="I4" s="18">
         <v>1.21952836700074</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="15"/>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="12"/>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6">
         <v>12</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6">
         <v>13</v>
       </c>
-      <c r="F5" s="6">
+      <c r="H5" s="6">
         <v>48</v>
       </c>
-      <c r="G5" s="6">
-        <v>12</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="I5" s="18">
         <v>9.8785349982790597E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="15"/>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="6">
+        <v>50</v>
+      </c>
+      <c r="F6" s="6">
         <v>101</v>
       </c>
-      <c r="E6" s="6">
+      <c r="G6" s="6">
         <v>271</v>
       </c>
-      <c r="F6" s="6">
+      <c r="H6" s="6">
         <v>414</v>
       </c>
-      <c r="G6" s="6">
-        <v>50</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="I6" s="18">
         <v>0.11152410300564899</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="15"/>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
         <v>55</v>
       </c>
-      <c r="E7" s="6">
+      <c r="G7" s="6">
         <v>57</v>
       </c>
-      <c r="F7" s="6">
+      <c r="H7" s="6">
         <v>224</v>
       </c>
-      <c r="G7" s="6">
-        <v>6</v>
-      </c>
-      <c r="H7" s="11">
+      <c r="I7" s="18">
         <v>4.2626645001291701E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="15"/>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
         <v>4229</v>
       </c>
-      <c r="E8" s="6">
+      <c r="G8" s="6">
         <v>4230</v>
       </c>
-      <c r="F8" s="6">
+      <c r="H8" s="6">
         <v>17029</v>
       </c>
-      <c r="G8" s="6">
-        <v>6</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="I8" s="18">
         <v>3.6028989160040501</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="22">
+        <v>6</v>
+      </c>
+      <c r="F9" s="22">
         <v>7</v>
       </c>
-      <c r="E9" s="6">
+      <c r="G9" s="22">
         <v>9</v>
       </c>
-      <c r="F9" s="6">
+      <c r="H9" s="22">
         <v>28</v>
       </c>
-      <c r="G9" s="6">
-        <v>6</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="I9" s="23">
         <v>8.5484230003203196E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6">
         <v>55</v>
       </c>
-      <c r="E10" s="6">
+      <c r="G10" s="6">
         <v>57</v>
       </c>
-      <c r="F10" s="6">
+      <c r="H10" s="6">
         <v>224</v>
       </c>
-      <c r="G10" s="6">
-        <v>6</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="I10" s="18">
         <v>4.90047790008247E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
         <v>41</v>
       </c>
-      <c r="E11" s="6">
+      <c r="G11" s="6">
         <v>43</v>
       </c>
-      <c r="F11" s="6">
+      <c r="H11" s="6">
         <v>170</v>
       </c>
-      <c r="G11" s="6">
-        <v>6</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="I11" s="18">
         <v>3.5959643006208297E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="15"/>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6</v>
+      </c>
+      <c r="F12" s="6">
         <v>11</v>
       </c>
-      <c r="E12" s="6">
+      <c r="G12" s="6">
         <v>13</v>
       </c>
-      <c r="F12" s="6">
+      <c r="H12" s="6">
         <v>50</v>
       </c>
-      <c r="G12" s="6">
-        <v>6</v>
-      </c>
-      <c r="H12" s="11">
+      <c r="I12" s="18">
         <v>1.13770153498626</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="17">
-        <f>AVERAGE(D3:D12)</f>
+      <c r="D13" s="17"/>
+      <c r="E13" s="14">
+        <f>AVERAGE(E3:E12)</f>
+        <v>11</v>
+      </c>
+      <c r="F13" s="14">
+        <f>AVERAGE(F3:F12)</f>
         <v>601.20000000000005</v>
       </c>
-      <c r="E13" s="9">
-        <f t="shared" ref="E13:H13" si="0">AVERAGE(E3:E12)</f>
+      <c r="G13" s="14">
+        <f t="shared" ref="G13:I13" si="0">AVERAGE(G3:G12)</f>
         <v>620.79999999999995</v>
       </c>
-      <c r="F13" s="17">
+      <c r="H13" s="14">
         <f t="shared" si="0"/>
         <v>2432.6999999999998</v>
       </c>
-      <c r="G13" s="17">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="H13" s="10">
+      <c r="I13" s="19">
         <f t="shared" si="0"/>
         <v>0.6258553995001408</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="G15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="H15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6</v>
+      </c>
+      <c r="F16" s="6">
         <v>205</v>
       </c>
-      <c r="E16" s="6">
+      <c r="G16" s="6">
         <v>337</v>
       </c>
-      <c r="F16" s="6">
+      <c r="H16" s="6">
         <v>1317</v>
       </c>
-      <c r="G16" s="6">
-        <v>6</v>
-      </c>
-      <c r="H16" s="11">
+      <c r="I16" s="18">
         <v>0.545943581004394</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6">
         <v>19747</v>
       </c>
-      <c r="E17" s="6">
+      <c r="G17" s="6">
         <v>19748</v>
       </c>
-      <c r="F17" s="6">
+      <c r="H17" s="6">
         <v>108950</v>
       </c>
-      <c r="G17" s="6">
-        <v>6</v>
-      </c>
-      <c r="H17" s="11">
+      <c r="I17" s="18">
         <v>41.108592712000203</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="15"/>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>9</v>
+      </c>
+      <c r="F18" s="6">
         <v>14</v>
       </c>
-      <c r="E18" s="6">
+      <c r="G18" s="6">
         <v>15</v>
       </c>
-      <c r="F18" s="6">
+      <c r="H18" s="6">
         <v>41</v>
       </c>
-      <c r="G18" s="6">
-        <v>9</v>
-      </c>
-      <c r="H18" s="11">
+      <c r="I18" s="18">
         <v>1.6682864006725098E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="12"/>
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <v>50</v>
+      </c>
+      <c r="F19" s="6">
         <v>1392</v>
       </c>
-      <c r="E19" s="6">
+      <c r="G19" s="6">
         <v>8572</v>
       </c>
-      <c r="F19" s="6">
+      <c r="H19" s="6">
         <v>8959</v>
       </c>
-      <c r="G19" s="6">
-        <v>50</v>
-      </c>
-      <c r="H19" s="11">
+      <c r="I19" s="18">
         <v>4.8224815459980102</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="15"/>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="12"/>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="F20" s="6">
         <v>387</v>
       </c>
-      <c r="E20" s="6">
+      <c r="G20" s="6">
         <v>389</v>
       </c>
-      <c r="F20" s="6">
+      <c r="H20" s="6">
         <v>2351</v>
       </c>
-      <c r="G20" s="6">
-        <v>6</v>
-      </c>
-      <c r="H20" s="11">
+      <c r="I20" s="18">
         <v>0.87828166900726501</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6">
         <v>84055</v>
       </c>
-      <c r="E21" s="6">
+      <c r="G21" s="6">
         <v>84056</v>
       </c>
-      <c r="F21" s="6">
+      <c r="H21" s="6">
         <v>445019</v>
       </c>
-      <c r="G21" s="6">
-        <v>6</v>
-      </c>
-      <c r="H21" s="11">
+      <c r="I21" s="18">
         <v>168.35773514299899</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="15"/>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
       <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
+        <v>10</v>
+      </c>
+      <c r="F22" s="6">
         <v>193</v>
       </c>
-      <c r="E22" s="6">
+      <c r="G22" s="6">
         <v>195</v>
       </c>
-      <c r="F22" s="6">
+      <c r="H22" s="6">
         <v>1026</v>
       </c>
-      <c r="G22" s="6">
-        <v>10</v>
-      </c>
-      <c r="H22" s="11">
+      <c r="I22" s="18">
         <v>0.39227325099636801</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="12"/>
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
         <v>387</v>
       </c>
-      <c r="E23" s="6">
+      <c r="G23" s="6">
         <v>389</v>
       </c>
-      <c r="F23" s="6">
+      <c r="H23" s="6">
         <v>2351</v>
       </c>
-      <c r="G23" s="6">
-        <v>6</v>
-      </c>
-      <c r="H23" s="11">
+      <c r="I23" s="18">
         <v>0.86623552899982303</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
-      <c r="C24" s="5" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="12"/>
+      <c r="C24" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="22">
+        <v>6</v>
+      </c>
+      <c r="F24" s="22">
         <v>108</v>
       </c>
-      <c r="E24" s="6">
+      <c r="G24" s="22">
         <v>110</v>
       </c>
-      <c r="F24" s="6">
+      <c r="H24" s="22">
         <v>761</v>
       </c>
-      <c r="G24" s="6">
-        <v>6</v>
-      </c>
-      <c r="H24" s="11">
+      <c r="I24" s="23">
         <v>0.28954632999375401</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="12"/>
       <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6">
         <v>35</v>
       </c>
-      <c r="E25" s="6">
+      <c r="G25" s="6">
         <v>37</v>
       </c>
-      <c r="F25" s="6">
+      <c r="H25" s="6">
         <v>192</v>
       </c>
-      <c r="G25" s="6">
-        <v>6</v>
-      </c>
-      <c r="H25" s="11">
+      <c r="I25" s="18">
         <v>33.2912620179995</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="9">
-        <f>AVERAGE(D16:D25)</f>
+      <c r="D26" s="17"/>
+      <c r="E26" s="14">
+        <f t="shared" ref="E26" si="1">AVERAGE(E16:E25)</f>
+        <v>11.1</v>
+      </c>
+      <c r="F26" s="14">
+        <f>AVERAGE(F16:F25)</f>
         <v>10652.3</v>
       </c>
-      <c r="E26" s="9">
-        <f t="shared" ref="E26" si="1">AVERAGE(E16:E25)</f>
+      <c r="G26" s="14">
+        <f t="shared" ref="G26" si="2">AVERAGE(G16:G25)</f>
         <v>11384.8</v>
       </c>
-      <c r="F26" s="17">
-        <f t="shared" ref="F26" si="2">AVERAGE(F16:F25)</f>
+      <c r="H26" s="14">
+        <f t="shared" ref="H26" si="3">AVERAGE(H16:H25)</f>
         <v>57096.7</v>
       </c>
-      <c r="G26" s="17">
-        <f t="shared" ref="G26" si="3">AVERAGE(G16:G25)</f>
-        <v>11.1</v>
-      </c>
-      <c r="H26" s="10">
-        <f t="shared" ref="H26" si="4">AVERAGE(H16:H25)</f>
+      <c r="I26" s="19">
+        <f t="shared" ref="I26" si="4">AVERAGE(I16:I25)</f>
         <v>25.0569034643005</v>
       </c>
     </row>
-    <row r="28" spans="2:8" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="G28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="H28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="14" t="s">
+      <c r="I28" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="15" t="s">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="6">
+        <v>12</v>
+      </c>
+      <c r="F29" s="6">
         <v>14491</v>
       </c>
-      <c r="E29" s="6">
+      <c r="G29" s="6">
         <v>17947</v>
       </c>
-      <c r="F29" s="6">
+      <c r="H29" s="6">
         <v>128184</v>
       </c>
-      <c r="G29" s="6">
-        <v>12</v>
-      </c>
-      <c r="H29" s="11">
+      <c r="I29" s="18">
         <v>131.446662653994</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="15"/>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="12"/>
       <c r="C30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="15"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="12"/>
       <c r="C31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1878</v>
+      </c>
+      <c r="F31" s="6">
         <v>1948</v>
       </c>
-      <c r="E31" s="6">
+      <c r="G31" s="6">
         <v>1949</v>
       </c>
-      <c r="F31" s="6">
+      <c r="H31" s="6">
         <v>16253</v>
       </c>
-      <c r="G31" s="6">
-        <v>1878</v>
-      </c>
-      <c r="H31" s="11">
+      <c r="I31" s="18">
         <v>26.679062017996301</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="15"/>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="12"/>
       <c r="C32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="15"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="12"/>
       <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="6">
+        <v>12</v>
+      </c>
+      <c r="F33" s="6">
         <v>17783</v>
       </c>
-      <c r="E33" s="6">
+      <c r="G33" s="6">
         <v>17785</v>
       </c>
-      <c r="F33" s="6">
+      <c r="H33" s="6">
         <v>155920</v>
       </c>
-      <c r="G33" s="6">
-        <v>12</v>
-      </c>
-      <c r="H33" s="11">
+      <c r="I33" s="18">
         <v>64.015925721003399</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="15"/>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="12"/>
       <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="15"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="12"/>
       <c r="C35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="6">
+        <v>22</v>
+      </c>
+      <c r="F35" s="6">
         <v>4031</v>
       </c>
-      <c r="E35" s="6">
+      <c r="G35" s="6">
         <v>4033</v>
       </c>
-      <c r="F35" s="6">
+      <c r="H35" s="6">
         <v>35794</v>
       </c>
-      <c r="G35" s="6">
-        <v>22</v>
-      </c>
-      <c r="H35" s="11">
+      <c r="I35" s="18">
         <v>15.8658084640046</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="15"/>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="12"/>
       <c r="C36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="6">
+        <v>12</v>
+      </c>
+      <c r="F36" s="6">
         <v>17783</v>
       </c>
-      <c r="E36" s="6">
+      <c r="G36" s="6">
         <v>17785</v>
       </c>
-      <c r="F36" s="6">
+      <c r="H36" s="6">
         <v>155920</v>
       </c>
-      <c r="G36" s="6">
+      <c r="I36" s="18">
+        <v>62.893093974998898</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
+      <c r="C37" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="22">
         <v>12</v>
       </c>
-      <c r="H36" s="11">
-        <v>62.893093974998898</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="15"/>
-      <c r="C37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="6">
+      <c r="F37" s="22">
         <v>5003</v>
       </c>
-      <c r="E37" s="6">
+      <c r="G37" s="22">
         <v>5005</v>
       </c>
-      <c r="F37" s="6">
+      <c r="H37" s="22">
         <v>44586</v>
       </c>
-      <c r="G37" s="6">
-        <v>12</v>
-      </c>
-      <c r="H37" s="11">
+      <c r="I37" s="23">
         <v>19.118624861992402</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="15"/>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="12"/>
       <c r="C38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="F38" s="16"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="6"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="2:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="8"/>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="9">
-        <f>AVERAGE(D29:D38)</f>
+      <c r="D39" s="17"/>
+      <c r="E39" s="14">
+        <f t="shared" ref="E39" si="5">AVERAGE(E29:E38)</f>
+        <v>324.66666666666669</v>
+      </c>
+      <c r="F39" s="14">
+        <f>AVERAGE(F29:F38)</f>
         <v>10173.166666666666</v>
       </c>
-      <c r="E39" s="9">
-        <f t="shared" ref="E39" si="5">AVERAGE(E29:E38)</f>
+      <c r="G39" s="14">
+        <f t="shared" ref="G39" si="6">AVERAGE(G29:G38)</f>
         <v>10750.666666666666</v>
       </c>
-      <c r="F39" s="17">
-        <f t="shared" ref="F39" si="6">AVERAGE(F29:F38)</f>
+      <c r="H39" s="14">
+        <f t="shared" ref="H39" si="7">AVERAGE(H29:H38)</f>
         <v>89442.833333333328</v>
       </c>
-      <c r="G39" s="17">
-        <f t="shared" ref="G39" si="7">AVERAGE(G29:G38)</f>
-        <v>324.66666666666669</v>
-      </c>
-      <c r="H39" s="10">
-        <f t="shared" ref="H39" si="8">AVERAGE(H29:H38)</f>
+      <c r="I39" s="19">
+        <f t="shared" ref="I39" si="8">AVERAGE(I29:I38)</f>
         <v>53.336529615664936</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug impacting p2 results
</commit_message>
<xml_diff>
--- a/ai-nano/projects/3-planning/results/data-table.xlsx
+++ b/ai-nano/projects/3-planning/results/data-table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18500" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
   <si>
     <t>Problem 1</t>
   </si>
@@ -269,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -337,6 +337,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -618,9 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -956,23 +963,21 @@
       <c r="C16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F16" s="6">
-        <v>205</v>
+        <v>3343</v>
       </c>
       <c r="G16" s="6">
-        <v>337</v>
+        <v>4609</v>
       </c>
       <c r="H16" s="6">
-        <v>1317</v>
+        <v>30509</v>
       </c>
       <c r="I16" s="18">
-        <v>0.545943581004394</v>
+        <v>16.798993903997999</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
@@ -980,24 +985,14 @@
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="6">
-        <v>6</v>
-      </c>
-      <c r="F17" s="6">
-        <v>19747</v>
-      </c>
-      <c r="G17" s="6">
-        <v>19748</v>
-      </c>
-      <c r="H17" s="6">
-        <v>108950</v>
-      </c>
-      <c r="I17" s="18">
-        <v>41.108592712000203</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
@@ -1006,19 +1001,19 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
-        <v>9</v>
+        <v>575</v>
       </c>
       <c r="F18" s="6">
-        <v>14</v>
+        <v>582</v>
       </c>
       <c r="G18" s="6">
-        <v>15</v>
+        <v>583</v>
       </c>
       <c r="H18" s="6">
-        <v>41</v>
+        <v>5211</v>
       </c>
       <c r="I18" s="18">
-        <v>1.6682864006725098E-2</v>
+        <v>3.72759502197732</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
@@ -1027,44 +1022,34 @@
         <v>4</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6">
-        <v>50</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1392</v>
-      </c>
-      <c r="G19" s="6">
-        <v>8572</v>
-      </c>
-      <c r="H19" s="6">
-        <v>8959</v>
-      </c>
-      <c r="I19" s="18">
-        <v>4.8224815459980102</v>
-      </c>
+      <c r="E19" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F20" s="6">
-        <v>387</v>
+        <v>4761</v>
       </c>
       <c r="G20" s="6">
-        <v>389</v>
+        <v>4763</v>
       </c>
       <c r="H20" s="6">
-        <v>2351</v>
+        <v>43206</v>
       </c>
       <c r="I20" s="18">
-        <v>0.87828166900726501</v>
+        <v>15.701451928995001</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
@@ -1072,24 +1057,14 @@
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="6">
-        <v>6</v>
-      </c>
-      <c r="F21" s="6">
-        <v>84055</v>
-      </c>
-      <c r="G21" s="6">
-        <v>84056</v>
-      </c>
-      <c r="H21" s="6">
-        <v>445019</v>
-      </c>
-      <c r="I21" s="18">
-        <v>168.35773514299899</v>
-      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
@@ -1098,19 +1073,19 @@
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="6">
-        <v>193</v>
+        <v>550</v>
       </c>
       <c r="G22" s="6">
-        <v>195</v>
+        <v>552</v>
       </c>
       <c r="H22" s="6">
-        <v>1026</v>
+        <v>4950</v>
       </c>
       <c r="I22" s="18">
-        <v>0.39227325099636801</v>
+        <v>1.73293168400414</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
@@ -1118,47 +1093,43 @@
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F23" s="6">
-        <v>387</v>
+        <v>4761</v>
       </c>
       <c r="G23" s="6">
-        <v>389</v>
+        <v>4763</v>
       </c>
       <c r="H23" s="6">
-        <v>2351</v>
+        <v>43206</v>
       </c>
       <c r="I23" s="18">
-        <v>0.86623552899982303</v>
+        <v>15.489678598009</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="22">
-        <v>6</v>
-      </c>
-      <c r="F24" s="22">
-        <v>108</v>
-      </c>
-      <c r="G24" s="22">
-        <v>110</v>
-      </c>
-      <c r="H24" s="22">
-        <v>761</v>
-      </c>
-      <c r="I24" s="23">
-        <v>0.28954632999375401</v>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26">
+        <v>9</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1450</v>
+      </c>
+      <c r="G24" s="26">
+        <v>1452</v>
+      </c>
+      <c r="H24" s="26">
+        <v>13303</v>
+      </c>
+      <c r="I24" s="27">
+        <v>4.6805308510083696</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
@@ -1166,24 +1137,14 @@
       <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="6">
-        <v>6</v>
-      </c>
-      <c r="F25" s="6">
-        <v>35</v>
-      </c>
-      <c r="G25" s="6">
-        <v>37</v>
-      </c>
-      <c r="H25" s="6">
-        <v>192</v>
-      </c>
-      <c r="I25" s="18">
-        <v>33.2912620179995</v>
-      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="2:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
@@ -1193,23 +1154,23 @@
       <c r="D26" s="17"/>
       <c r="E26" s="14">
         <f t="shared" ref="E26" si="1">AVERAGE(E16:E25)</f>
-        <v>11.1</v>
+        <v>103.33333333333333</v>
       </c>
       <c r="F26" s="14">
         <f>AVERAGE(F16:F25)</f>
-        <v>10652.3</v>
+        <v>2574.5</v>
       </c>
       <c r="G26" s="14">
         <f t="shared" ref="G26" si="2">AVERAGE(G16:G25)</f>
-        <v>11384.8</v>
+        <v>2787</v>
       </c>
       <c r="H26" s="14">
         <f t="shared" ref="H26" si="3">AVERAGE(H16:H25)</f>
-        <v>57096.7</v>
+        <v>23397.5</v>
       </c>
       <c r="I26" s="19">
         <f t="shared" ref="I26" si="4">AVERAGE(I16:I25)</f>
-        <v>25.0569034643005</v>
+        <v>9.6885303313319717</v>
       </c>
     </row>
     <row r="28" spans="2:9" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>